<commit_message>
Updated error message for IDA
</commit_message>
<xml_diff>
--- a/docs/requirements/Requirements Detailing References/ID-Authentication/Sprint FIT-4/Consolidated error messages V2.3.xlsx
+++ b/docs/requirements/Requirements Detailing References/ID-Authentication/Sprint FIT-4/Consolidated error messages V2.3.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MOSIP\Project\error message\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MOSIPRequirementsGithub\docs\requirements\Requirements Detailing References\ID-Authentication\Sprint FIT-4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{00A40933-F132-4B4F-BB88-E1CB3157790F}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{90CF19DD-B6B4-4F28-98F4-2D6EAB3CBB5F}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9675" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -780,9 +780,6 @@
     <t>“Partner is unauthorised for eKYC”</t>
   </si>
   <si>
-    <t>“Unable to decrypt Authentication Request.”</t>
-  </si>
-  <si>
     <t>Invalid encryption of session key/request</t>
   </si>
   <si>
@@ -919,9 +916,6 @@
   </si>
   <si>
     <t>“Input transactionID does not match transactionID of OTP Request”</t>
-  </si>
-  <si>
-    <t>Could not process request/Unknown error; Invalid Auth Request; Failure in Decryption</t>
   </si>
   <si>
     <t>PartnerID is not mapped to a policy</t>
@@ -1144,6 +1138,12 @@
   </si>
   <si>
     <t>IDA-MLC-018</t>
+  </si>
+  <si>
+    <t>Could not process request/Unknown error; Invalid Auth Request</t>
+  </si>
+  <si>
+    <t>“Unable to decrypt Request.”</t>
   </si>
 </sst>
 </file>
@@ -1775,8 +1775,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="19.7109375" defaultRowHeight="28.5" customHeight="1" outlineLevelCol="1" x14ac:dyDescent="0.2"/>
@@ -1811,7 +1811,7 @@
         <v>8</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="2" spans="1:12" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -1903,19 +1903,19 @@
         <v>5</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="E6" s="6" t="s">
         <v>24</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="G6" s="8"/>
     </row>
@@ -2029,7 +2029,7 @@
         <v>45</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="D12" s="6"/>
       <c r="E12" s="6"/>
@@ -2055,12 +2055,12 @@
       </c>
       <c r="G13" s="8"/>
     </row>
-    <row r="14" spans="1:12" ht="63" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:12" ht="47.25" x14ac:dyDescent="0.2">
       <c r="A14" s="4">
         <v>13</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>252</v>
+        <v>297</v>
       </c>
       <c r="C14" s="6" t="s">
         <v>119</v>
@@ -2072,21 +2072,21 @@
       </c>
       <c r="G14" s="8"/>
     </row>
-    <row r="15" spans="1:12" ht="63" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:12" ht="78.75" x14ac:dyDescent="0.2">
       <c r="A15" s="4">
         <v>14</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="D15" s="6" t="s">
         <v>209</v>
       </c>
       <c r="E15" s="6" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="F15" s="6" t="s">
         <v>48</v>
@@ -2107,14 +2107,14 @@
         <v>114</v>
       </c>
       <c r="E16" s="6" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="F16" s="6" t="s">
         <v>53</v>
       </c>
       <c r="G16" s="8"/>
     </row>
-    <row r="17" spans="1:7" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7" ht="47.25" x14ac:dyDescent="0.2">
       <c r="A17" s="4">
         <v>16</v>
       </c>
@@ -2133,7 +2133,7 @@
       </c>
       <c r="G17" s="8"/>
     </row>
-    <row r="18" spans="1:7" ht="78.75" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7" ht="94.5" x14ac:dyDescent="0.2">
       <c r="A18" s="4">
         <v>17</v>
       </c>
@@ -2146,7 +2146,7 @@
       <c r="D18" s="6"/>
       <c r="E18" s="6"/>
       <c r="F18" s="6" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="G18" s="8"/>
     </row>
@@ -2166,7 +2166,7 @@
         <v>57</v>
       </c>
       <c r="G19" s="21" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="31.5" x14ac:dyDescent="0.2">
@@ -2180,13 +2180,13 @@
         <v>210</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="E20" s="6" t="s">
         <v>49</v>
       </c>
       <c r="F20" s="22" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="G20" s="8"/>
     </row>
@@ -2195,13 +2195,13 @@
         <v>20</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="C21" s="6" t="s">
+        <v>263</v>
+      </c>
+      <c r="D21" s="6" t="s">
         <v>265</v>
-      </c>
-      <c r="D21" s="6" t="s">
-        <v>267</v>
       </c>
       <c r="E21" s="6" t="s">
         <v>52</v>
@@ -2225,10 +2225,10 @@
         <v>66</v>
       </c>
       <c r="E22" s="6" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="F22" s="6" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="G22" s="8"/>
     </row>
@@ -2240,7 +2240,7 @@
         <v>71</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="D23" s="6"/>
       <c r="E23" s="6"/>
@@ -2254,15 +2254,15 @@
         <v>24</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="C24" s="6" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="D24" s="16"/>
       <c r="E24" s="6"/>
       <c r="F24" s="6" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="G24" s="8"/>
     </row>
@@ -2271,10 +2271,10 @@
         <v>25</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="D25" s="16"/>
       <c r="E25" s="6"/>
@@ -2291,13 +2291,13 @@
         <v>79</v>
       </c>
       <c r="C26" s="6" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="D26" s="6" t="s">
         <v>92</v>
       </c>
       <c r="E26" s="6" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="F26" s="6" t="s">
         <v>72</v>
@@ -2333,7 +2333,7 @@
         <v>84</v>
       </c>
       <c r="C28" s="6" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="D28" s="6"/>
       <c r="E28" s="6"/>
@@ -2350,12 +2350,12 @@
         <v>85</v>
       </c>
       <c r="C29" s="6" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="D29" s="6"/>
       <c r="E29" s="6"/>
       <c r="F29" s="6" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="G29" s="8"/>
     </row>
@@ -2372,7 +2372,7 @@
       <c r="D30" s="6"/>
       <c r="E30" s="6"/>
       <c r="F30" s="6" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="G30" s="6">
         <v>2</v>
@@ -2433,15 +2433,15 @@
       <c r="A34" s="4">
         <v>40</v>
       </c>
-      <c r="B34" s="6" t="s">
-        <v>223</v>
-      </c>
-      <c r="C34" s="6" t="s">
+      <c r="B34" s="19" t="s">
         <v>222</v>
       </c>
-      <c r="D34" s="6"/>
-      <c r="E34" s="6"/>
-      <c r="F34" s="6" t="s">
+      <c r="C34" s="19" t="s">
+        <v>298</v>
+      </c>
+      <c r="D34" s="19"/>
+      <c r="E34" s="19"/>
+      <c r="F34" s="19" t="s">
         <v>185</v>
       </c>
       <c r="G34" s="8"/>
@@ -2451,10 +2451,10 @@
         <v>41</v>
       </c>
       <c r="B35" s="5" t="s">
+        <v>246</v>
+      </c>
+      <c r="C35" s="5" t="s">
         <v>247</v>
-      </c>
-      <c r="C35" s="5" t="s">
-        <v>248</v>
       </c>
       <c r="D35" s="20"/>
       <c r="E35" s="20"/>
@@ -2491,7 +2491,7 @@
       <c r="D37" s="8"/>
       <c r="E37" s="8"/>
       <c r="F37" s="6" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="G37" s="8"/>
     </row>
@@ -2508,7 +2508,7 @@
       <c r="D38" s="8"/>
       <c r="E38" s="8"/>
       <c r="F38" s="6" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="G38" s="8"/>
     </row>
@@ -2537,10 +2537,10 @@
         <v>101</v>
       </c>
       <c r="C40" s="6" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="D40" s="16" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="E40" s="6" t="s">
         <v>59</v>
@@ -2575,7 +2575,7 @@
         <v>109</v>
       </c>
       <c r="C42" s="6" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D42" s="6"/>
       <c r="E42" s="6"/>
@@ -2676,7 +2676,7 @@
         <v>197</v>
       </c>
       <c r="G47" s="21" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="H47" s="12"/>
       <c r="I47" s="12"/>
@@ -2692,7 +2692,7 @@
         <v>190</v>
       </c>
       <c r="C48" s="5" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="D48" s="6"/>
       <c r="E48" s="6"/>
@@ -2706,10 +2706,10 @@
         <v>56</v>
       </c>
       <c r="B49" s="6" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C49" s="5" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="D49" s="6"/>
       <c r="E49" s="6"/>
@@ -2723,7 +2723,7 @@
         <v>57</v>
       </c>
       <c r="B50" s="6" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="C50" s="6" t="s">
         <v>198</v>
@@ -2777,7 +2777,7 @@
         <v>203</v>
       </c>
       <c r="C53" s="6" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="D53" s="6"/>
       <c r="E53" s="6"/>
@@ -2791,7 +2791,7 @@
         <v>61</v>
       </c>
       <c r="B54" s="6" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="C54" s="6" t="s">
         <v>204</v>
@@ -2811,7 +2811,7 @@
         <v>205</v>
       </c>
       <c r="C55" s="6" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="D55" s="6"/>
       <c r="E55" s="6"/>
@@ -2842,10 +2842,10 @@
         <v>64</v>
       </c>
       <c r="B57" s="6" t="s">
+        <v>248</v>
+      </c>
+      <c r="C57" s="6" t="s">
         <v>249</v>
-      </c>
-      <c r="C57" s="6" t="s">
-        <v>250</v>
       </c>
       <c r="D57" s="6"/>
       <c r="E57" s="6"/>
@@ -2859,10 +2859,10 @@
         <v>63</v>
       </c>
       <c r="B58" s="6" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="C58" s="5" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="D58" s="6"/>
       <c r="E58" s="6"/>
@@ -2876,15 +2876,15 @@
         <v>64</v>
       </c>
       <c r="B59" s="6" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="C59" s="5" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="D59" s="6"/>
       <c r="E59" s="6"/>
       <c r="F59" s="6" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="G59" s="8"/>
     </row>
@@ -2893,15 +2893,15 @@
         <v>65</v>
       </c>
       <c r="B60" s="6" t="s">
+        <v>257</v>
+      </c>
+      <c r="C60" s="6" t="s">
         <v>259</v>
-      </c>
-      <c r="C60" s="6" t="s">
-        <v>261</v>
       </c>
       <c r="D60" s="6"/>
       <c r="E60" s="6"/>
       <c r="F60" s="8" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="G60" s="8"/>
     </row>
@@ -2910,15 +2910,15 @@
         <v>66</v>
       </c>
       <c r="B61" s="6" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="C61" s="6" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="D61" s="8"/>
       <c r="E61" s="6"/>
       <c r="F61" s="6" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="G61" s="6"/>
     </row>
@@ -2930,7 +2930,7 @@
         <v>68</v>
       </c>
       <c r="C62" s="21" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="D62" s="21" t="s">
         <v>69</v>
@@ -2965,15 +2965,15 @@
         <v>66</v>
       </c>
       <c r="B64" s="6" t="s">
+        <v>269</v>
+      </c>
+      <c r="C64" s="6" t="s">
         <v>271</v>
-      </c>
-      <c r="C64" s="6" t="s">
-        <v>273</v>
       </c>
       <c r="D64" s="6"/>
       <c r="E64" s="8"/>
       <c r="F64" s="8" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="G64" s="7"/>
     </row>
@@ -2982,15 +2982,15 @@
         <v>67</v>
       </c>
       <c r="B65" s="6" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="C65" s="6" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="D65" s="6"/>
       <c r="E65" s="6"/>
       <c r="F65" s="8" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="G65" s="7"/>
     </row>
@@ -2999,15 +2999,15 @@
         <v>68</v>
       </c>
       <c r="B66" s="6" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="C66" s="6" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="D66" s="6"/>
       <c r="E66" s="17"/>
       <c r="F66" s="6" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="G66" s="6"/>
     </row>
@@ -3016,15 +3016,15 @@
         <v>69</v>
       </c>
       <c r="B67" s="19" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="C67" s="19" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="D67" s="19"/>
       <c r="E67" s="26"/>
       <c r="F67" s="19" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="G67" s="19"/>
     </row>
@@ -3351,13 +3351,13 @@
         <v>21</v>
       </c>
       <c r="B22" s="18" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="C22" s="18" t="s">
+        <v>287</v>
+      </c>
+      <c r="D22" s="18" t="s">
         <v>289</v>
-      </c>
-      <c r="D22" s="18" t="s">
-        <v>291</v>
       </c>
     </row>
   </sheetData>

</xml_diff>